<commit_message>
add new siteparts kind
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -17,7 +17,7 @@
     <x:sheet name="バナー" sheetId="10" r:id="rId10"/>
     <x:sheet name="バナー種別" sheetId="11" r:id="rId11"/>
     <x:sheet name="関連ページ" sheetId="12" r:id="rId12"/>
-    <x:sheet name="商品ページ関連" sheetId="13" r:id="rId13"/>
+    <x:sheet name="陳列商品" sheetId="13" r:id="rId13"/>
     <x:sheet name="検索情報" sheetId="14" r:id="rId14"/>
   </x:sheets>
   <x:definedNames/>
@@ -424,7 +424,7 @@
     <x:t>RelateCode =&gt; Code</x:t>
   </x:si>
   <x:si>
-    <x:t>商品ページ関連</x:t>
+    <x:t>陳列商品</x:t>
   </x:si>
   <x:si>
     <x:t>ProductRelations</x:t>
@@ -1322,7 +1322,7 @@
     <x:hyperlink ref="A9" location="'バナー'!A1" display="バナー"/>
     <x:hyperlink ref="A10" location="'バナー種別'!A1" display="バナー種別"/>
     <x:hyperlink ref="A11" location="'関連ページ'!A1" display="関連ページ"/>
-    <x:hyperlink ref="A12" location="'商品ページ関連'!A1" display="商品ページ関連"/>
+    <x:hyperlink ref="A12" location="'陳列商品'!A1" display="陳列商品"/>
     <x:hyperlink ref="A13" location="'検索情報'!A1" display="検索情報"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -2641,7 +2641,7 @@
         <x:v>84</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>49</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s"/>
       <x:c r="E11" s="3" t="s">

</xml_diff>